<commit_message>
excel reader and used in test
</commit_message>
<xml_diff>
--- a/src/test/java/resources/LoginDetails.xlsx
+++ b/src/test/java/resources/LoginDetails.xlsx
@@ -23,66 +23,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Booster</author>
-  </authors>
-  <commentList>
-    <comment ref="A4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Booster:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Logically valid password is not applicable here, but pass a correct password which should available in Database or used for active user.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Booster:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-blank password is same as invalid password, but check the error messages should display proper text. (not generic programme for invalid and blank)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>EmailID</t>
   </si>
@@ -102,66 +44,35 @@
     <t>Invalid</t>
   </si>
   <si>
-    <t>Scenario</t>
-  </si>
-  <si>
-    <t>Valid email id , valid password</t>
-  </si>
-  <si>
-    <t>Valid emailid, Invalid password</t>
-  </si>
-  <si>
-    <t>Invalid emali id, valid password</t>
-  </si>
-  <si>
-    <t>Invalid emaild, invalid password</t>
-  </si>
-  <si>
-    <t>Valid email id , blank password</t>
-  </si>
-  <si>
     <t>email@emaikl.com</t>
   </si>
   <si>
     <t>mypassword</t>
   </si>
   <si>
-    <t>thepassiswrong</t>
-  </si>
-  <si>
-    <t>Eitehr email or password is incorrect</t>
-  </si>
-  <si>
-    <t>invalid_email</t>
-  </si>
-  <si>
-    <t>invalid_pass</t>
+    <t/>
+  </si>
+  <si>
+    <t>Invalid Login Credentials.</t>
+  </si>
+  <si>
+    <t>chamtester23@gmail.com</t>
+  </si>
+  <si>
+    <t>Welcome@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <u/>
@@ -171,16 +82,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -188,14 +113,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -476,116 +420,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>